<commit_message>
PDF reports to excel convertion
</commit_message>
<xml_diff>
--- a/AlgaehReporting/algaeh_report_tool/templates/Excel/nationalityWiseEmployee.xlsx
+++ b/AlgaehReporting/algaeh_report_tool/templates/Excel/nationalityWiseEmployee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/ALGAEH/DEV/hims-app-merged/AlgaehReporting/algaeh_report_tool/templates/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665C9741-C2F6-7547-B664-3E67B418064A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552784C6-3710-D846-8779-E5918F414E1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="1460" windowWidth="27640" windowHeight="16540" xr2:uid="{12465D96-D6FD-674D-8DDE-9A106529BC26}"/>
   </bookViews>
@@ -69,10 +69,10 @@
     <t>EMP. STATUS</t>
   </si>
   <si>
-    <t>${table:data.nationality}</t>
-  </si>
-  <si>
-    <t>${table:data.no_employee}</t>
+    <t>${table:result.nationality}</t>
+  </si>
+  <si>
+    <t>${table:result.no_employee}</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A2:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J7" sqref="J7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>